<commit_message>
Fixed up template with more instructions.
</commit_message>
<xml_diff>
--- a/March 30 Weekly Report.xlsx
+++ b/March 30 Weekly Report.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
   <si>
     <t>Name</t>
   </si>
@@ -113,6 +113,11 @@
 * Calculate Ownership of Component
 *Calculate Issues vs ownership per month
 *Calculate Issues vs ownership in general</t>
+  </si>
+  <si>
+    <t>*Excel statistics may not accurately reflect seasonal/holiday commits vs issues due to some holidays being on the edge of months (Christmas/New years)
+*
+*</t>
   </si>
 </sst>
 </file>
@@ -565,10 +570,10 @@
   <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomRight" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -677,7 +682,7 @@
       </c>
       <c r="F5" s="3"/>
     </row>
-    <row r="6" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="120" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>14</v>
       </c>
@@ -691,7 +696,7 @@
         <v>26</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="F6" s="3"/>
     </row>

</xml_diff>